<commit_message>
Database Update; add views Coupler's and Pole kit's
</commit_message>
<xml_diff>
--- a/equipment.xlsx
+++ b/equipment.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$G$806</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$G$855</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -5481,7 +5481,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G855"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A821" workbookViewId="0">
+      <selection activeCell="L851" sqref="L851"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -25155,7 +25157,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G806"/>
+  <autoFilter ref="A1:G855"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>